<commit_message>
added 'set_name_space' modified vendor input card
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>CWE</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>Time and State:Insecure Temporary File</t>
+  </si>
+  <si>
+    <t>Line_Number</t>
+  </si>
+  <si>
+    <t>ClassInfo/line</t>
   </si>
 </sst>
 </file>
@@ -829,21 +835,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="62.06640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="62.06640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="7.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="62" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="50.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -863,7 +869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>78</v>
       </c>
@@ -875,7 +881,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>90</v>
       </c>
@@ -887,7 +893,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>121</v>
       </c>
@@ -903,7 +909,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>122</v>
       </c>
@@ -919,7 +925,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>123</v>
       </c>
@@ -928,7 +934,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>124</v>
       </c>
@@ -938,7 +944,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>126</v>
       </c>
@@ -952,7 +958,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>127</v>
       </c>
@@ -962,7 +968,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>134</v>
       </c>
@@ -976,7 +982,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>176</v>
       </c>
@@ -988,7 +994,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>188</v>
       </c>
@@ -1000,7 +1006,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>190</v>
       </c>
@@ -1014,7 +1020,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>191</v>
       </c>
@@ -1024,7 +1030,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>194</v>
       </c>
@@ -1040,7 +1046,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>195</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>196</v>
       </c>
@@ -1070,7 +1076,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>197</v>
       </c>
@@ -1080,7 +1086,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>242</v>
       </c>
@@ -1092,7 +1098,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>369</v>
       </c>
@@ -1102,7 +1108,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>377</v>
       </c>
@@ -1114,7 +1120,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>400</v>
       </c>
@@ -1126,7 +1132,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>401</v>
       </c>
@@ -1140,7 +1146,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>404</v>
       </c>
@@ -1152,7 +1158,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>415</v>
       </c>
@@ -1164,7 +1170,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>416</v>
       </c>
@@ -1176,7 +1182,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>426</v>
       </c>
@@ -1188,7 +1194,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>427</v>
       </c>
@@ -1198,7 +1204,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>457</v>
       </c>
@@ -1210,7 +1216,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>459</v>
       </c>
@@ -1220,7 +1226,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>464</v>
       </c>
@@ -1230,7 +1236,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>467</v>
       </c>
@@ -1240,7 +1246,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>468</v>
       </c>
@@ -1252,7 +1258,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>469</v>
       </c>
@@ -1262,7 +1268,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>475</v>
       </c>
@@ -1274,7 +1280,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>476</v>
       </c>
@@ -1288,7 +1294,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>562</v>
       </c>
@@ -1300,7 +1306,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>587</v>
       </c>
@@ -1310,7 +1316,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>588</v>
       </c>
@@ -1320,7 +1326,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>590</v>
       </c>
@@ -1332,7 +1338,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>665</v>
       </c>
@@ -1344,7 +1350,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>675</v>
       </c>
@@ -1354,7 +1360,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>680</v>
       </c>
@@ -1366,7 +1372,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>681</v>
       </c>
@@ -1376,7 +1382,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>690</v>
       </c>
@@ -1388,7 +1394,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>758</v>
       </c>
@@ -1398,7 +1404,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>761</v>
       </c>
@@ -1410,7 +1416,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>773</v>
       </c>
@@ -1422,7 +1428,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>775</v>
       </c>
@@ -1434,7 +1440,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>785</v>
       </c>
@@ -1446,7 +1452,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>789</v>
       </c>
@@ -1456,7 +1462,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>843</v>
       </c>
@@ -1476,20 +1482,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>48</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>54</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>56</v>
       </c>
@@ -1552,6 +1558,17 @@
         <v>57</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1565,18 +1582,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.53125" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="12"/>
+    <col min="1" max="1" width="1.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12">
         <v>1</v>
       </c>
@@ -1584,7 +1601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>2</v>
       </c>
@@ -1592,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>3</v>
       </c>
@@ -1600,7 +1617,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
partially implemented new parser
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>CWE</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>Time and State:Insecure Temporary File</t>
+  </si>
+  <si>
+    <t>Line_Number</t>
+  </si>
+  <si>
+    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/line</t>
   </si>
 </sst>
 </file>
@@ -829,18 +835,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="62.06640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="62.06640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
     <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -1476,17 +1482,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -1524,21 +1530,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>50</v>
@@ -1546,12 +1552,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1565,15 +1582,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.53125" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="12"/>
+    <col min="2" max="2" width="255.59765625" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
updated reading from xml tags
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -355,9 +355,6 @@
     <t>Tag or Attribute</t>
   </si>
   <si>
-    <t>Finding_type</t>
-  </si>
-  <si>
     <t>Vulnerabilities/Vulnerability</t>
   </si>
   <si>
@@ -391,7 +388,10 @@
     <t>Line_Number</t>
   </si>
   <si>
-    <t>ClassInfo/line</t>
+    <t>AnalysisInfo/Unified/Context/FunctionDeclarationSourceLocation/line</t>
+  </si>
+  <si>
+    <t>Finding_Type</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1113,7 @@
         <v>377</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1485,14 +1485,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,13 +1508,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1522,54 +1522,54 @@
         <v>34</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All TURE scores now match previous version
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ws3 duplicate files now highlighted as expected
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
@@ -835,21 +835,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
     <col min="2" max="2" width="62" style="5" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -869,7 +869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="8">
         <v>78</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="8">
         <v>90</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="8">
         <v>121</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="8">
         <v>122</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="8">
         <v>123</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="8">
         <v>124</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="8">
         <v>126</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="8">
         <v>127</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="8">
         <v>134</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="8">
         <v>176</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="8">
         <v>188</v>
       </c>
@@ -1006,7 +1006,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="8">
         <v>190</v>
       </c>
@@ -1020,7 +1020,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="8">
         <v>191</v>
       </c>
@@ -1030,7 +1030,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="8">
         <v>194</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="8">
         <v>195</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="8">
         <v>196</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="8">
         <v>197</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="8">
         <v>242</v>
       </c>
@@ -1098,7 +1098,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="8">
         <v>369</v>
       </c>
@@ -1108,7 +1108,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="8">
         <v>377</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="8">
         <v>400</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="8">
         <v>401</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="8">
         <v>404</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="8">
         <v>415</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="8">
         <v>416</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="8">
         <v>426</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="8">
         <v>427</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="8">
         <v>457</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="8">
         <v>459</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="8">
         <v>464</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="8">
         <v>467</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <v>468</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="8">
         <v>469</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="8">
         <v>475</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="8">
         <v>476</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="8">
         <v>562</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="8">
         <v>587</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="8">
         <v>588</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="8">
         <v>590</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="8">
         <v>665</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="8">
         <v>675</v>
       </c>
@@ -1360,7 +1360,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="8">
         <v>680</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="8">
         <v>681</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="8">
         <v>690</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="8">
         <v>758</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="8">
         <v>761</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="8">
         <v>773</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="8">
         <v>775</v>
       </c>
@@ -1440,7 +1440,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="8">
         <v>785</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="8">
         <v>789</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="8">
         <v>843</v>
       </c>
@@ -1488,14 +1488,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>53</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>55</v>
       </c>
@@ -1586,14 +1586,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.59765625" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12">
         <v>1</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
         <v>2</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
         <v>3</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
ws3 highlighting working as expected
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -835,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1484,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1582,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add new enclosing function to vi sheet
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>CWE</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>Finding_Type</t>
+  </si>
+  <si>
+    <t>Function_Name</t>
+  </si>
+  <si>
+    <t>AnalysisInfo/Unified/Context/Function/name</t>
   </si>
 </sst>
 </file>
@@ -839,17 +845,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="9" customWidth="1"/>
     <col min="2" max="2" width="62" style="5" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="50.5703125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -869,7 +875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>78</v>
       </c>
@@ -881,7 +887,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>90</v>
       </c>
@@ -893,7 +899,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>121</v>
       </c>
@@ -909,7 +915,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>122</v>
       </c>
@@ -925,7 +931,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>123</v>
       </c>
@@ -934,7 +940,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>124</v>
       </c>
@@ -944,7 +950,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>126</v>
       </c>
@@ -958,7 +964,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>127</v>
       </c>
@@ -968,7 +974,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>134</v>
       </c>
@@ -982,7 +988,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>176</v>
       </c>
@@ -994,7 +1000,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>188</v>
       </c>
@@ -1006,7 +1012,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>190</v>
       </c>
@@ -1020,7 +1026,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>191</v>
       </c>
@@ -1030,7 +1036,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>194</v>
       </c>
@@ -1046,7 +1052,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>195</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>196</v>
       </c>
@@ -1076,7 +1082,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>197</v>
       </c>
@@ -1086,7 +1092,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>242</v>
       </c>
@@ -1098,7 +1104,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>369</v>
       </c>
@@ -1108,7 +1114,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>377</v>
       </c>
@@ -1120,7 +1126,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>400</v>
       </c>
@@ -1132,7 +1138,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>401</v>
       </c>
@@ -1146,7 +1152,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>404</v>
       </c>
@@ -1158,7 +1164,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>415</v>
       </c>
@@ -1170,7 +1176,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>416</v>
       </c>
@@ -1182,7 +1188,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>426</v>
       </c>
@@ -1194,7 +1200,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>427</v>
       </c>
@@ -1204,7 +1210,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>457</v>
       </c>
@@ -1216,7 +1222,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>459</v>
       </c>
@@ -1226,7 +1232,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>464</v>
       </c>
@@ -1236,7 +1242,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>467</v>
       </c>
@@ -1246,7 +1252,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>468</v>
       </c>
@@ -1258,7 +1264,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>469</v>
       </c>
@@ -1268,7 +1274,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>475</v>
       </c>
@@ -1280,7 +1286,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>476</v>
       </c>
@@ -1294,7 +1300,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>562</v>
       </c>
@@ -1306,7 +1312,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>587</v>
       </c>
@@ -1316,7 +1322,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>588</v>
       </c>
@@ -1326,7 +1332,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>590</v>
       </c>
@@ -1338,7 +1344,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>665</v>
       </c>
@@ -1350,7 +1356,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>675</v>
       </c>
@@ -1360,7 +1366,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>680</v>
       </c>
@@ -1372,7 +1378,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>681</v>
       </c>
@@ -1382,7 +1388,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>690</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>758</v>
       </c>
@@ -1404,7 +1410,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>761</v>
       </c>
@@ -1416,7 +1422,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>773</v>
       </c>
@@ -1428,7 +1434,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>775</v>
       </c>
@@ -1440,7 +1446,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>785</v>
       </c>
@@ -1452,7 +1458,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>789</v>
       </c>
@@ -1462,7 +1468,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>843</v>
       </c>
@@ -1482,20 +1488,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1539,36 +1545,47 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1582,18 +1599,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.59765625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12">
         <v>1</v>
       </c>
@@ -1601,7 +1618,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>2</v>
       </c>
@@ -1609,7 +1626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>3</v>
       </c>
@@ -1617,7 +1634,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
general update prior to implementing new method for calculating the opp counts via test case object __init__
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
@@ -841,21 +841,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
     <col min="2" max="2" width="62" style="5" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -875,7 +875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="8">
         <v>78</v>
       </c>
@@ -887,7 +887,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="8">
         <v>90</v>
       </c>
@@ -899,7 +899,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="8">
         <v>121</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="8">
         <v>122</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="8">
         <v>123</v>
       </c>
@@ -940,7 +940,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="8">
         <v>124</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="8">
         <v>126</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="8">
         <v>127</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="8">
         <v>134</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="8">
         <v>176</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="8">
         <v>188</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="8">
         <v>190</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="8">
         <v>191</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="8">
         <v>194</v>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="8">
         <v>195</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="8">
         <v>196</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="8">
         <v>197</v>
       </c>
@@ -1092,7 +1092,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="8">
         <v>242</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="8">
         <v>369</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="8">
         <v>377</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="8">
         <v>400</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="8">
         <v>401</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="8">
         <v>404</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="8">
         <v>415</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="8">
         <v>416</v>
       </c>
@@ -1188,7 +1188,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="8">
         <v>426</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="8">
         <v>427</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="8">
         <v>457</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="8">
         <v>459</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="8">
         <v>464</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="8">
         <v>467</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <v>468</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="8">
         <v>469</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="8">
         <v>475</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="8">
         <v>476</v>
       </c>
@@ -1300,7 +1300,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="8">
         <v>562</v>
       </c>
@@ -1312,7 +1312,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="8">
         <v>587</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="8">
         <v>588</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="8">
         <v>590</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="8">
         <v>665</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="8">
         <v>675</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="8">
         <v>680</v>
       </c>
@@ -1378,7 +1378,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="8">
         <v>681</v>
       </c>
@@ -1388,7 +1388,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="8">
         <v>690</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="8">
         <v>758</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="8">
         <v>761</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="8">
         <v>773</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="8">
         <v>775</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="8">
         <v>785</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="8">
         <v>789</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="8">
         <v>843</v>
       </c>
@@ -1490,18 +1490,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>60</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>61</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>36</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>53</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -1603,14 +1603,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.59765625" style="12" customWidth="1"/>
     <col min="3" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12">
         <v>1</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
         <v>2</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
         <v>3</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
wid coloring on ws2 now completed and shows used=green and unused=red
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -440,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,15 +509,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,6 +516,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,12 +848,12 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="12" customWidth="1"/>
     <col min="2" max="2" width="62" style="5" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
@@ -855,28 +861,28 @@
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="8">
+      <c r="A2" s="14">
         <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -888,7 +894,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
+      <c r="A3" s="14">
         <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -900,7 +906,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="8">
+      <c r="A4" s="14">
         <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -916,7 +922,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
+      <c r="A5" s="14">
         <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -932,7 +938,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="8">
+      <c r="A6" s="14">
         <v>123</v>
       </c>
       <c r="C6" s="3"/>
@@ -941,7 +947,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="8">
+      <c r="A7" s="14">
         <v>124</v>
       </c>
       <c r="B7" s="2"/>
@@ -951,7 +957,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="8">
+      <c r="A8" s="14">
         <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -965,7 +971,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="8">
+      <c r="A9" s="14">
         <v>127</v>
       </c>
       <c r="B9" s="2"/>
@@ -975,7 +981,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="8">
+      <c r="A10" s="14">
         <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -989,7 +995,7 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="8">
+      <c r="A11" s="14">
         <v>176</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1001,7 +1007,7 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="8">
+      <c r="A12" s="14">
         <v>188</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1013,7 +1019,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="8">
+      <c r="A13" s="14">
         <v>190</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1027,7 +1033,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="8">
+      <c r="A14" s="14">
         <v>191</v>
       </c>
       <c r="B14" s="2"/>
@@ -1037,7 +1043,7 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="8">
+      <c r="A15" s="14">
         <v>194</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1053,7 +1059,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="8">
+      <c r="A16" s="14">
         <v>195</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1073,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="8">
+      <c r="A17" s="14">
         <v>196</v>
       </c>
       <c r="B17" s="2"/>
@@ -1083,7 +1089,7 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="8">
+      <c r="A18" s="14">
         <v>197</v>
       </c>
       <c r="B18" s="2"/>
@@ -1093,7 +1099,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="8">
+      <c r="A19" s="14">
         <v>242</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1105,7 +1111,7 @@
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="8">
+      <c r="A20" s="14">
         <v>369</v>
       </c>
       <c r="B20" s="2"/>
@@ -1115,7 +1121,7 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="8">
+      <c r="A21" s="14">
         <v>377</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1127,7 +1133,7 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="8">
+      <c r="A22" s="14">
         <v>400</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1139,7 +1145,7 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="8">
+      <c r="A23" s="14">
         <v>401</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1153,7 +1159,7 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="8">
+      <c r="A24" s="14">
         <v>404</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1165,7 +1171,7 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="8">
+      <c r="A25" s="14">
         <v>415</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1177,7 +1183,7 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="8">
+      <c r="A26" s="14">
         <v>416</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1189,7 +1195,7 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="8">
+      <c r="A27" s="14">
         <v>426</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1201,7 +1207,7 @@
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="8">
+      <c r="A28" s="14">
         <v>427</v>
       </c>
       <c r="B28" s="2"/>
@@ -1211,7 +1217,7 @@
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="8">
+      <c r="A29" s="14">
         <v>457</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1223,7 +1229,7 @@
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="8">
+      <c r="A30" s="14">
         <v>459</v>
       </c>
       <c r="B30" s="2"/>
@@ -1233,7 +1239,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="8">
+      <c r="A31" s="14">
         <v>464</v>
       </c>
       <c r="B31" s="2"/>
@@ -1243,7 +1249,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="8">
+      <c r="A32" s="14">
         <v>467</v>
       </c>
       <c r="B32" s="2"/>
@@ -1253,7 +1259,7 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="8">
+      <c r="A33" s="14">
         <v>468</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1265,7 +1271,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="8">
+      <c r="A34" s="14">
         <v>469</v>
       </c>
       <c r="B34" s="2"/>
@@ -1275,7 +1281,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="8">
+      <c r="A35" s="14">
         <v>475</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1287,7 +1293,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="8">
+      <c r="A36" s="14">
         <v>476</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1301,7 +1307,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="8">
+      <c r="A37" s="14">
         <v>562</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1313,7 +1319,7 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="8">
+      <c r="A38" s="14">
         <v>587</v>
       </c>
       <c r="B38" s="2"/>
@@ -1323,7 +1329,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="8">
+      <c r="A39" s="14">
         <v>588</v>
       </c>
       <c r="B39" s="2"/>
@@ -1333,7 +1339,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="8">
+      <c r="A40" s="14">
         <v>590</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1345,7 +1351,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="8">
+      <c r="A41" s="14">
         <v>665</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1357,7 +1363,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="8">
+      <c r="A42" s="14">
         <v>675</v>
       </c>
       <c r="B42" s="2"/>
@@ -1367,7 +1373,7 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="8">
+      <c r="A43" s="14">
         <v>680</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1379,7 +1385,7 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="8">
+      <c r="A44" s="14">
         <v>681</v>
       </c>
       <c r="B44" s="2"/>
@@ -1389,7 +1395,7 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="8">
+      <c r="A45" s="14">
         <v>690</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1401,7 +1407,7 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="8">
+      <c r="A46" s="14">
         <v>758</v>
       </c>
       <c r="B46" s="2"/>
@@ -1411,7 +1417,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="8">
+      <c r="A47" s="14">
         <v>761</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1423,7 +1429,7 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="8">
+      <c r="A48" s="14">
         <v>773</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1435,7 +1441,7 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="8">
+      <c r="A49" s="14">
         <v>775</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1447,7 +1453,7 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="8">
+      <c r="A50" s="14">
         <v>785</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1459,7 +1465,7 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="8">
+      <c r="A51" s="14">
         <v>789</v>
       </c>
       <c r="B51" s="2"/>
@@ -1469,7 +1475,7 @@
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="8">
+      <c r="A52" s="14">
         <v>843</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1502,43 +1508,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1546,10 +1552,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1557,35 +1563,35 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1605,37 +1611,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.59765625" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="12"/>
+    <col min="1" max="1" width="1.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.59765625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="12">
+      <c r="A1" s="9">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 'SCORE' tab, recall-only chart on ws1, and other general cleanup
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="468" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weakness IDs" sheetId="2" r:id="rId1"/>
     <sheet name="XML Tags" sheetId="5" r:id="rId2"/>
     <sheet name="Scan Commands" sheetId="4" r:id="rId3"/>
+    <sheet name="Vendor Info" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>CWE</t>
   </si>
@@ -398,6 +399,33 @@
   </si>
   <si>
     <t>AnalysisInfo/Unified/Context/Function/name</t>
+  </si>
+  <si>
+    <t>Vendor Name:</t>
+  </si>
+  <si>
+    <t>Date of Scan:</t>
+  </si>
+  <si>
+    <t>Scan Conductor:</t>
+  </si>
+  <si>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t>Tool Version:</t>
+  </si>
+  <si>
+    <t>Rule Pack Version:</t>
+  </si>
+  <si>
+    <t>Rules Implemented:</t>
+  </si>
+  <si>
+    <t>Tool Name:</t>
+  </si>
+  <si>
+    <t>HP Fortify</t>
   </si>
 </sst>
 </file>
@@ -440,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,37 +527,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,644 +892,645 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="A72" sqref="A71:F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="62" style="5" customWidth="1"/>
-    <col min="3" max="3" width="62" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.59765625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.59765625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="7.3984375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="62" style="19" customWidth="1"/>
+    <col min="3" max="3" width="62" style="17" customWidth="1"/>
+    <col min="4" max="4" width="60.59765625" style="17" customWidth="1"/>
+    <col min="5" max="6" width="50.59765625" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="14">
+      <c r="A2" s="5">
         <v>78</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="14">
+      <c r="A3" s="5">
         <v>90</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="14">
+      <c r="A4" s="5">
         <v>121</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="14">
+      <c r="A5" s="5">
         <v>122</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="14">
+      <c r="A6" s="5">
         <v>123</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="14">
+      <c r="A7" s="5">
         <v>124</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="14">
+      <c r="A8" s="5">
         <v>126</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="14">
+      <c r="A9" s="5">
         <v>127</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="14">
+      <c r="A10" s="5">
         <v>134</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="14">
+      <c r="A11" s="5">
         <v>176</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="14">
+      <c r="A12" s="5">
         <v>188</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="14">
+      <c r="A13" s="5">
         <v>190</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="14">
+      <c r="A14" s="5">
         <v>191</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="14">
+      <c r="A15" s="5">
         <v>194</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="14">
+      <c r="A16" s="5">
         <v>195</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="14">
+      <c r="A17" s="5">
         <v>196</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="14">
+      <c r="A18" s="5">
         <v>197</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="14">
+      <c r="A19" s="5">
         <v>242</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="14">
+      <c r="A20" s="5">
         <v>369</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="14">
+      <c r="A21" s="5">
         <v>377</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="14">
+      <c r="A22" s="5">
         <v>400</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="14">
+      <c r="A23" s="5">
         <v>401</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="14">
+      <c r="A24" s="5">
         <v>404</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="14">
+      <c r="A25" s="5">
         <v>415</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="14">
+      <c r="A26" s="5">
         <v>416</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="14">
+      <c r="A27" s="5">
         <v>426</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="14">
+      <c r="A28" s="5">
         <v>427</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="14">
+      <c r="A29" s="5">
         <v>457</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="14">
+      <c r="A30" s="5">
         <v>459</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="14">
+      <c r="A31" s="5">
         <v>464</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="14">
+      <c r="A32" s="5">
         <v>467</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="14">
+      <c r="A33" s="5">
         <v>468</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="14">
+      <c r="A34" s="5">
         <v>469</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="14">
+      <c r="A35" s="5">
         <v>475</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="14">
+      <c r="A36" s="5">
         <v>476</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="14">
+      <c r="A37" s="5">
         <v>562</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="14">
+      <c r="A38" s="5">
         <v>587</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="14">
+      <c r="A39" s="5">
         <v>588</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="14">
+      <c r="A40" s="5">
         <v>590</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="14">
+      <c r="A41" s="5">
         <v>665</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="14">
+      <c r="A42" s="5">
         <v>675</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="14">
+      <c r="A43" s="5">
         <v>680</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="14">
+      <c r="A44" s="5">
         <v>681</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="14">
+      <c r="A45" s="5">
         <v>690</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="14">
+      <c r="A46" s="5">
         <v>758</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="14">
+      <c r="A47" s="5">
         <v>761</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="14">
+      <c r="A48" s="5">
         <v>773</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="14">
+      <c r="A49" s="5">
         <v>775</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="14">
+      <c r="A50" s="5">
         <v>785</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="14">
+      <c r="A51" s="5">
         <v>789</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="14">
+      <c r="A52" s="5">
         <v>843</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1496,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1508,90 +1554,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1605,43 +1651,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.59765625" style="9" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="1.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.59765625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="9">
+      <c r="A1" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="9">
+      <c r="A2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1649,4 +1695,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.46484375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.19921875" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" ht="234.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
general updates preparing for addition of data to 'SCORE' sheet
</commit_message>
<xml_diff>
--- a/vendor-input-fortify-c.xlsx
+++ b/vendor-input-fortify-c.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>CWE</t>
   </si>
@@ -426,6 +426,15 @@
   </si>
   <si>
     <t>HP Fortify</t>
+  </si>
+  <si>
+    <t>Language:</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Contact (email):</t>
   </si>
 </sst>
 </file>
@@ -1699,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1744,23 +1753,37 @@
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:2" ht="234.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:2" ht="234.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>